<commit_message>
Refactored agent tools on test setup
</commit_message>
<xml_diff>
--- a/setup/recyclinghof.xlsx
+++ b/setup/recyclinghof.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nghho\OneDrive\Desktop\Masterarbeit\dev\Native\WasteSeparationChatbotLLM\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904563E7-DF88-4294-A63A-5A44734CFC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A894C6C-8FF7-4B9D-8510-C3C9082B75FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,10 +51,6 @@
     <t>Kalbach-Riedberg</t>
   </si>
   <si>
-    <t>- Sommeröffnungszeiten: (01.04. – 30.09.): Mo.–Sa. 8.00–17.00 Uhr
-- Winteröffnungszeiten: (01.10. – 31.03.): Mo.–Sa. 10.00–16.00 Uhr</t>
-  </si>
-  <si>
     <t>FES-Wertstoffhof Nord</t>
   </si>
   <si>
@@ -76,19 +72,12 @@
     <t>Sachsenhausen</t>
   </si>
   <si>
-    <t>- Öffnungszeiten: Mo.–Sa. 8.00–14.30 Uhr</t>
-  </si>
-  <si>
     <t>Breuerwiesenstraße 2</t>
   </si>
   <si>
     <t>Höchst</t>
   </si>
   <si>
-    <t>- Sommeröffnungszeiten (01.04. – 30.09.): Mo.–Sa. 8.00–17.00 Uhr
-- Winteröffnungszeiten (01.10. – 31.03.): Mo.–Sa. 10.00–16.00 Uhr</t>
-  </si>
-  <si>
     <t>60596</t>
   </si>
   <si>
@@ -99,6 +88,17 @@
   </si>
   <si>
     <t>65929</t>
+  </si>
+  <si>
+    <t>Sommeröffnungszeiten: (01.04. – 30.09.): Mo.–Sa. 8.00–17.00 Uhr
+Winteröffnungszeiten: (01.10. – 31.03.): Mo.–Sa. 10.00–16.00 Uhr</t>
+  </si>
+  <si>
+    <t>Öffnungszeiten: Mo.–Sa. 8.00–14.30 Uhr</t>
+  </si>
+  <si>
+    <t>Sommeröffnungszeiten (01.04. – 30.09.): Mo.–Sa. 8.00–17.00 Uhr
+Winteröffnungszeiten (01.10. – 31.03.): Mo.–Sa. 10.00–16.00 Uhr</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +422,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="Q5" sqref="A1:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +431,7 @@
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -445,25 +447,25 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -471,50 +473,50 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -522,56 +524,56 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>